<commit_message>
feat: pagination invoices page, detail pages
</commit_message>
<xml_diff>
--- a/backend/orders/Production Sheet.xlsx
+++ b/backend/orders/Production Sheet.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="32">
   <si>
     <t>Ascent production Sheet</t>
   </si>
@@ -72,6 +72,9 @@
   </si>
   <si>
     <t>Polish:</t>
+  </si>
+  <si>
+    <t>Color:</t>
   </si>
   <si>
     <t>Rhodium:</t>
@@ -306,7 +309,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="38">
+  <fills count="39">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -322,6 +325,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0" tint="-0.0499893185216834"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.05"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -660,7 +669,7 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -684,16 +693,16 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="8" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="9" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="9" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="10" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="9" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="10" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="10" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="11" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
@@ -702,89 +711,89 @@
     <xf numFmtId="0" fontId="17" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="22" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="22" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="22" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="22" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="22" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="22" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="38" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -809,6 +818,9 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -820,7 +832,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -830,10 +842,10 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1158,7 +1170,7 @@
   <dimension ref="A1:H33"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14:D14"/>
+      <selection activeCell="B15" sqref="B15:D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="18" outlineLevelCol="7"/>
@@ -1274,7 +1286,9 @@
       <c r="A9" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="C9" s="3"/>
+      <c r="C9" s="10" t="s">
+        <v>15</v>
+      </c>
       <c r="E9" s="2"/>
       <c r="F9" s="2"/>
       <c r="G9" s="2"/>
@@ -1282,9 +1296,9 @@
     </row>
     <row r="10" spans="1:8">
       <c r="A10" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="C10" s="10"/>
+        <v>16</v>
+      </c>
+      <c r="C10" s="11"/>
       <c r="E10" s="2"/>
       <c r="F10" s="2"/>
       <c r="G10" s="2"/>
@@ -1292,9 +1306,9 @@
     </row>
     <row r="11" spans="1:8">
       <c r="A11" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="C11" s="10"/>
+        <v>17</v>
+      </c>
+      <c r="C11" s="11"/>
       <c r="E11" s="2"/>
       <c r="F11" s="2"/>
       <c r="G11" s="2"/>
@@ -1302,10 +1316,10 @@
     </row>
     <row r="12" spans="1:8">
       <c r="A12" s="4" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B12" s="6"/>
-      <c r="C12" s="11"/>
+      <c r="C12" s="12"/>
       <c r="D12" s="6"/>
       <c r="E12" s="2"/>
       <c r="F12" s="2"/>
@@ -1324,11 +1338,11 @@
     </row>
     <row r="14" spans="1:8">
       <c r="A14" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="B14" s="12"/>
-      <c r="C14" s="12"/>
-      <c r="D14" s="12"/>
+        <v>19</v>
+      </c>
+      <c r="B14" s="13"/>
+      <c r="C14" s="13"/>
+      <c r="D14" s="13"/>
       <c r="E14" s="2"/>
       <c r="F14" s="2"/>
       <c r="G14" s="2"/>
@@ -1336,11 +1350,11 @@
     </row>
     <row r="15" spans="1:8">
       <c r="A15" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="B15" s="12"/>
-      <c r="C15" s="12"/>
-      <c r="D15" s="12"/>
+        <v>20</v>
+      </c>
+      <c r="B15" s="13"/>
+      <c r="C15" s="13"/>
+      <c r="D15" s="13"/>
       <c r="E15" s="2"/>
       <c r="F15" s="2"/>
       <c r="G15" s="2"/>
@@ -1348,7 +1362,7 @@
     </row>
     <row r="16" spans="1:8">
       <c r="A16" s="7" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B16" s="2"/>
       <c r="C16" s="2"/>
@@ -1360,7 +1374,7 @@
     </row>
     <row r="17" spans="1:8">
       <c r="A17" s="8" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B17" s="8"/>
       <c r="C17" s="8"/>
@@ -1371,182 +1385,182 @@
       <c r="H17" s="8"/>
     </row>
     <row r="18" spans="1:8">
-      <c r="A18" s="13"/>
-      <c r="B18" s="14"/>
-      <c r="C18" s="14"/>
-      <c r="D18" s="14"/>
-      <c r="E18" s="14"/>
-      <c r="F18" s="14"/>
-      <c r="G18" s="14"/>
-      <c r="H18" s="14"/>
+      <c r="A18" s="14"/>
+      <c r="B18" s="15"/>
+      <c r="C18" s="15"/>
+      <c r="D18" s="15"/>
+      <c r="E18" s="15"/>
+      <c r="F18" s="15"/>
+      <c r="G18" s="15"/>
+      <c r="H18" s="15"/>
     </row>
     <row r="19" spans="1:8">
-      <c r="A19" s="14"/>
-      <c r="B19" s="14"/>
-      <c r="C19" s="14"/>
-      <c r="D19" s="14"/>
-      <c r="E19" s="14"/>
-      <c r="F19" s="14"/>
-      <c r="G19" s="14"/>
-      <c r="H19" s="14"/>
+      <c r="A19" s="15"/>
+      <c r="B19" s="15"/>
+      <c r="C19" s="15"/>
+      <c r="D19" s="15"/>
+      <c r="E19" s="15"/>
+      <c r="F19" s="15"/>
+      <c r="G19" s="15"/>
+      <c r="H19" s="15"/>
     </row>
     <row r="20" spans="1:8">
-      <c r="A20" s="14"/>
-      <c r="B20" s="14"/>
-      <c r="C20" s="14"/>
-      <c r="D20" s="14"/>
-      <c r="E20" s="14"/>
-      <c r="F20" s="14"/>
-      <c r="G20" s="14"/>
-      <c r="H20" s="14"/>
+      <c r="A20" s="15"/>
+      <c r="B20" s="15"/>
+      <c r="C20" s="15"/>
+      <c r="D20" s="15"/>
+      <c r="E20" s="15"/>
+      <c r="F20" s="15"/>
+      <c r="G20" s="15"/>
+      <c r="H20" s="15"/>
     </row>
     <row r="21" spans="1:8">
-      <c r="A21" s="14"/>
-      <c r="B21" s="14"/>
-      <c r="C21" s="14"/>
-      <c r="D21" s="14"/>
-      <c r="E21" s="14"/>
-      <c r="F21" s="14"/>
-      <c r="G21" s="14"/>
-      <c r="H21" s="14"/>
+      <c r="A21" s="15"/>
+      <c r="B21" s="15"/>
+      <c r="C21" s="15"/>
+      <c r="D21" s="15"/>
+      <c r="E21" s="15"/>
+      <c r="F21" s="15"/>
+      <c r="G21" s="15"/>
+      <c r="H21" s="15"/>
     </row>
     <row r="22" spans="1:8">
-      <c r="A22" s="14"/>
-      <c r="B22" s="14"/>
-      <c r="C22" s="14"/>
-      <c r="D22" s="14"/>
-      <c r="E22" s="14"/>
-      <c r="F22" s="14"/>
-      <c r="G22" s="14"/>
-      <c r="H22" s="14"/>
+      <c r="A22" s="15"/>
+      <c r="B22" s="15"/>
+      <c r="C22" s="15"/>
+      <c r="D22" s="15"/>
+      <c r="E22" s="15"/>
+      <c r="F22" s="15"/>
+      <c r="G22" s="15"/>
+      <c r="H22" s="15"/>
     </row>
     <row r="23" ht="14" customHeight="1" spans="1:8">
-      <c r="A23" s="14"/>
-      <c r="B23" s="14"/>
-      <c r="C23" s="14"/>
-      <c r="D23" s="14"/>
-      <c r="E23" s="14"/>
-      <c r="F23" s="14"/>
-      <c r="G23" s="14"/>
-      <c r="H23" s="14"/>
+      <c r="A23" s="15"/>
+      <c r="B23" s="15"/>
+      <c r="C23" s="15"/>
+      <c r="D23" s="15"/>
+      <c r="E23" s="15"/>
+      <c r="F23" s="15"/>
+      <c r="G23" s="15"/>
+      <c r="H23" s="15"/>
     </row>
     <row r="24" ht="21" spans="1:8">
-      <c r="A24" s="15" t="s">
-        <v>22</v>
-      </c>
-      <c r="B24" s="15"/>
-      <c r="C24" s="15"/>
-      <c r="D24" s="15"/>
-      <c r="E24" s="15"/>
-      <c r="F24" s="15"/>
-      <c r="G24" s="15"/>
-      <c r="H24" s="15"/>
+      <c r="A24" s="16" t="s">
+        <v>23</v>
+      </c>
+      <c r="B24" s="16"/>
+      <c r="C24" s="16"/>
+      <c r="D24" s="16"/>
+      <c r="E24" s="16"/>
+      <c r="F24" s="16"/>
+      <c r="G24" s="16"/>
+      <c r="H24" s="16"/>
     </row>
     <row r="25" spans="1:8">
-      <c r="A25" s="16" t="s">
-        <v>23</v>
-      </c>
-      <c r="B25" s="16" t="s">
+      <c r="A25" s="17" t="s">
         <v>24</v>
       </c>
-      <c r="C25" s="16" t="s">
+      <c r="B25" s="17" t="s">
         <v>25</v>
       </c>
-      <c r="D25" s="16" t="s">
+      <c r="C25" s="17" t="s">
         <v>26</v>
       </c>
-      <c r="E25" s="16" t="s">
+      <c r="D25" s="17" t="s">
         <v>27</v>
       </c>
-      <c r="F25" s="16" t="s">
+      <c r="E25" s="17" t="s">
         <v>28</v>
       </c>
-      <c r="G25" s="16" t="s">
+      <c r="F25" s="17" t="s">
         <v>29</v>
       </c>
-      <c r="H25" s="16" t="s">
+      <c r="G25" s="17" t="s">
         <v>30</v>
+      </c>
+      <c r="H25" s="17" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="26" spans="1:8">
       <c r="A26" s="4"/>
-      <c r="B26" s="17"/>
+      <c r="B26" s="18"/>
       <c r="C26" s="4"/>
-      <c r="D26" s="18"/>
-      <c r="E26" s="18"/>
-      <c r="F26" s="18"/>
-      <c r="G26" s="18"/>
-      <c r="H26" s="18"/>
+      <c r="D26" s="19"/>
+      <c r="E26" s="19"/>
+      <c r="F26" s="19"/>
+      <c r="G26" s="19"/>
+      <c r="H26" s="19"/>
     </row>
     <row r="27" spans="1:8">
-      <c r="A27" s="19"/>
-      <c r="B27" s="19"/>
-      <c r="C27" s="19"/>
-      <c r="D27" s="20"/>
-      <c r="E27" s="20"/>
-      <c r="F27" s="20"/>
-      <c r="G27" s="20"/>
-      <c r="H27" s="20"/>
+      <c r="A27" s="20"/>
+      <c r="B27" s="20"/>
+      <c r="C27" s="20"/>
+      <c r="D27" s="21"/>
+      <c r="E27" s="21"/>
+      <c r="F27" s="21"/>
+      <c r="G27" s="21"/>
+      <c r="H27" s="21"/>
     </row>
     <row r="28" spans="1:8">
       <c r="A28" s="4"/>
       <c r="B28" s="4"/>
       <c r="C28" s="4"/>
-      <c r="D28" s="18"/>
-      <c r="E28" s="18"/>
+      <c r="D28" s="19"/>
+      <c r="E28" s="19"/>
       <c r="F28" s="4"/>
       <c r="G28" s="4"/>
       <c r="H28" s="4"/>
     </row>
     <row r="29" spans="1:8">
-      <c r="A29" s="19"/>
-      <c r="B29" s="19"/>
-      <c r="C29" s="19"/>
-      <c r="D29" s="20"/>
-      <c r="E29" s="20"/>
-      <c r="F29" s="19"/>
-      <c r="G29" s="19"/>
-      <c r="H29" s="19"/>
+      <c r="A29" s="20"/>
+      <c r="B29" s="20"/>
+      <c r="C29" s="20"/>
+      <c r="D29" s="21"/>
+      <c r="E29" s="21"/>
+      <c r="F29" s="20"/>
+      <c r="G29" s="20"/>
+      <c r="H29" s="20"/>
     </row>
     <row r="30" spans="1:8">
       <c r="A30" s="4"/>
       <c r="B30" s="4"/>
       <c r="C30" s="4"/>
-      <c r="D30" s="18"/>
-      <c r="E30" s="18"/>
+      <c r="D30" s="19"/>
+      <c r="E30" s="19"/>
       <c r="F30" s="4"/>
       <c r="G30" s="4"/>
       <c r="H30" s="4"/>
     </row>
     <row r="31" spans="1:8">
-      <c r="A31" s="19"/>
-      <c r="B31" s="19"/>
-      <c r="C31" s="19"/>
-      <c r="D31" s="20"/>
-      <c r="E31" s="20"/>
-      <c r="F31" s="19"/>
-      <c r="G31" s="19"/>
-      <c r="H31" s="19"/>
+      <c r="A31" s="20"/>
+      <c r="B31" s="20"/>
+      <c r="C31" s="20"/>
+      <c r="D31" s="21"/>
+      <c r="E31" s="21"/>
+      <c r="F31" s="20"/>
+      <c r="G31" s="20"/>
+      <c r="H31" s="20"/>
     </row>
     <row r="32" spans="1:8">
       <c r="A32" s="4"/>
       <c r="B32" s="4"/>
       <c r="C32" s="4"/>
-      <c r="D32" s="18"/>
-      <c r="E32" s="18"/>
+      <c r="D32" s="19"/>
+      <c r="E32" s="19"/>
       <c r="F32" s="4"/>
       <c r="G32" s="4"/>
       <c r="H32" s="4"/>
     </row>
     <row r="33" spans="1:8">
-      <c r="A33" s="19"/>
-      <c r="B33" s="19"/>
-      <c r="C33" s="19"/>
-      <c r="D33" s="20"/>
-      <c r="E33" s="20"/>
-      <c r="F33" s="19"/>
-      <c r="G33" s="19"/>
-      <c r="H33" s="19"/>
+      <c r="A33" s="20"/>
+      <c r="B33" s="20"/>
+      <c r="C33" s="20"/>
+      <c r="D33" s="21"/>
+      <c r="E33" s="21"/>
+      <c r="F33" s="20"/>
+      <c r="G33" s="20"/>
+      <c r="H33" s="20"/>
     </row>
   </sheetData>
   <mergeCells count="10">

</xml_diff>